<commit_message>
getting ready for the next paper
</commit_message>
<xml_diff>
--- a/data/aineisto_2023.xlsx
+++ b/data/aineisto_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anttitanskanen/Github/Syntyvyyden-tekij-t/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77805E72-E656-6541-8495-49C4925E25CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760C5003-DDBE-1049-A5AF-1906CCF1B94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="760" windowWidth="21540" windowHeight="17700" xr2:uid="{7A7B6AD2-3A7D-5D45-9F88-9535E8DFA96B}"/>
+    <workbookView xWindow="360" yWindow="760" windowWidth="21540" windowHeight="17700" xr2:uid="{7A7B6AD2-3A7D-5D45-9F88-9535E8DFA96B}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul2" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="syntyvyysaineisto_CHECK2023" localSheetId="0">Taul2!$A$1:$AZ$43</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2244,7 +2244,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="alypuhelin"/>
@@ -3237,8 +3237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5873E55E-AD10-E54B-ABAD-63D2E5A9C7F1}">
   <dimension ref="A1:AZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3607,7 +3607,7 @@
         <v>1.79</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E35" si="0">D3</f>
+        <f t="shared" ref="E3:E30" si="0">D3</f>
         <v>1.79</v>
       </c>
       <c r="F3">

</xml_diff>